<commit_message>
Added performance related and highly ranked (1-14) bugs
</commit_message>
<xml_diff>
--- a/StaticAnalysis.xlsx
+++ b/StaticAnalysis.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="45">
   <si>
     <t>Identifier of defect</t>
   </si>
@@ -33,9 +33,6 @@
   </si>
   <si>
     <t>Rank</t>
-  </si>
-  <si>
-    <t>A known null value is checked to see if it is an instance of a type</t>
   </si>
   <si>
     <t>Description</t>
@@ -56,14 +53,110 @@
     <t>Impact</t>
   </si>
   <si>
+    <t>No impact</t>
+  </si>
+  <si>
+    <t>Nullcheck of value previously dereferenced</t>
+  </si>
+  <si>
+    <t>A value is checked here to see whether it is null, but this value can't be null because it was previously dereferenced and if it were null a null pointer exception would have occurred at the earlier dereference. Essentially, this code and the previous dereference disagree as to whether this value is allowed to be null. Either the check is redundant or the previous dereference is erroneous.</t>
+  </si>
+  <si>
+    <t>A known null value is checked to see if it is an instance of a type in sh.world.shworld.SpaceHulkWorldModel line 569</t>
+  </si>
+  <si>
+    <t>A known null value is checked to see if it is an instance of a type in sh.agent.door.DoorModel line 586</t>
+  </si>
+  <si>
+    <t>True Positive</t>
+  </si>
+  <si>
+    <t>The warning is true. We can safely remove the redundant check as the same check has been done in line 633</t>
+  </si>
+  <si>
+    <t>Comparison of String objects using == or !=</t>
+  </si>
+  <si>
+    <t>This code compares java.lang.String objects for reference equality using the == or != operators. Unless both strings are either constants in a source file, or have been interned using the String.intern() method, the same string value may be represented by two different String objects. Consider using the equals(Object) method instead.</t>
+  </si>
+  <si>
+    <t>The warning is true.</t>
+  </si>
+  <si>
+    <t>Message description</t>
+  </si>
+  <si>
+    <t>Little or no impact.</t>
+  </si>
+  <si>
+    <t>BY message description</t>
+  </si>
+  <si>
+    <t>Unwritten field</t>
+  </si>
+  <si>
+    <t>This field is never written.  All reads of it will return the default value. Check for errors (should it have been initialized?), or remove it if it is useless.</t>
+  </si>
+  <si>
+    <t>Undecided</t>
+  </si>
+  <si>
+    <t>The warning make sense</t>
+  </si>
+  <si>
+    <t>Message description and code view</t>
+  </si>
+  <si>
+    <t>Should be a static inner class</t>
+  </si>
+  <si>
+    <t>This class is an inner class, but does not use its embedded reference to the object which created it.  This reference makes the instances of the class larger, and may keep the reference to the creator object alive longer than necessary.  If possible, the class should be made static.</t>
+  </si>
+  <si>
+    <t>The warning makes sense</t>
+  </si>
+  <si>
+    <t>Little impact</t>
+  </si>
+  <si>
+    <t>Private method is never called</t>
+  </si>
+  <si>
+    <t>This private method is never called. Although it is possible that the method will be invoked through reflection, it is more likely that the method is never used, and should be removed.</t>
+  </si>
+  <si>
+    <t>The warning makes sense. The piece of code can be removed.</t>
+  </si>
+  <si>
     <t>No or very little impact</t>
+  </si>
+  <si>
+    <t>Unread field</t>
+  </si>
+  <si>
+    <t>This field is never read.  Consider removing it from the class.</t>
+  </si>
+  <si>
+    <t>Unused field</t>
+  </si>
+  <si>
+    <t>This field is never used.  Consider removing it from the class.</t>
+  </si>
+  <si>
+    <t>Scary Bugs</t>
+  </si>
+  <si>
+    <t>Troubling Bugs</t>
+  </si>
+  <si>
+    <t>Performance Related Bugs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -92,6 +185,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -113,7 +213,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -136,6 +236,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -452,7 +555,7 @@
   <sheetData>
     <row r="2" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -658,14 +761,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G572"/>
+  <dimension ref="A1:G583"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
     <col min="2" max="2" width="37.28515625" style="4" customWidth="1"/>
     <col min="3" max="3" width="50" customWidth="1"/>
     <col min="4" max="4" width="19.28515625" customWidth="1"/>
@@ -687,45 +791,48 @@
         <v>2</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+    </row>
+    <row r="3" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="5" t="s">
+      <c r="F3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>8</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B3" s="3"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B4" s="3"/>
@@ -735,13 +842,25 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B5" s="3"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+    <row r="5" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="B5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" s="3"/>
@@ -752,6 +871,9 @@
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>43</v>
+      </c>
       <c r="B7" s="3"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -759,13 +881,28 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B8" s="3"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+    <row r="8" spans="1:7" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>11</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B9" s="3"/>
@@ -775,13 +912,25 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B10" s="3"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+    <row r="10" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="B10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B11" s="3"/>
@@ -791,13 +940,25 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B12" s="3"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+    <row r="12" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="B12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B13" s="3"/>
@@ -807,13 +968,25 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B14" s="3"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+    <row r="14" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="B14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B15" s="3"/>
@@ -823,15 +996,27 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B16" s="3"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="B16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B17" s="3"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -839,15 +1024,27 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B18" s="3"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="B18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B19" s="3"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -855,15 +1052,27 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B20" s="3"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="B20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B21" s="3"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -871,15 +1080,30 @@
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B22" s="3"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>12</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B23" s="3"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -887,7 +1111,10 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A24" s="7" t="s">
+        <v>44</v>
+      </c>
       <c r="B24" s="3"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -895,7 +1122,7 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B25" s="3"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -903,15 +1130,30 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B26" s="3"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>18</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B27" s="3"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -919,15 +1161,27 @@
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B28" s="3"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="B28" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B29" s="3"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -935,15 +1189,27 @@
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B30" s="3"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="B30" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B31" s="3"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -951,13 +1217,25 @@
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B32" s="3"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
+    <row r="32" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="B32" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B33" s="3"/>
@@ -967,13 +1245,25 @@
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B34" s="3"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
+    <row r="34" spans="2:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="B34" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B35" s="3"/>
@@ -983,13 +1273,25 @@
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B36" s="3"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
+    <row r="36" spans="2:7" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B36" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B37" s="3"/>
@@ -999,13 +1301,25 @@
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B38" s="3"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
+    <row r="38" spans="2:7" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B38" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B39" s="3"/>
@@ -1015,13 +1329,25 @@
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B40" s="3"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
+    <row r="40" spans="2:7" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B40" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B41" s="3"/>
@@ -1031,13 +1357,25 @@
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
     </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B42" s="3"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
+    <row r="42" spans="2:7" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B42" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B43" s="3"/>
@@ -1047,13 +1385,25 @@
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B44" s="3"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
+    <row r="44" spans="2:7" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B44" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B45" s="3"/>
@@ -1063,13 +1413,25 @@
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
     </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B46" s="3"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
+    <row r="46" spans="2:7" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B46" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B47" s="3"/>
@@ -1079,13 +1441,25 @@
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
     </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B48" s="3"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
+    <row r="48" spans="2:7" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B48" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B49" s="3"/>
@@ -1095,13 +1469,25 @@
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B50" s="3"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
+    <row r="50" spans="2:7" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B50" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B51" s="3"/>
@@ -1111,13 +1497,25 @@
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B52" s="3"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
+    <row r="52" spans="2:7" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B52" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B53" s="3"/>
@@ -1127,13 +1525,25 @@
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
     </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B54" s="3"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
+    <row r="54" spans="2:7" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B54" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B55" s="3"/>
@@ -1143,13 +1553,25 @@
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
     </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B56" s="3"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
+    <row r="56" spans="2:7" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B56" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B57" s="3"/>
@@ -1159,13 +1581,25 @@
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B58" s="3"/>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
+    <row r="58" spans="2:7" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B58" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B59" s="3"/>
@@ -1175,13 +1609,25 @@
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
     </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B60" s="3"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
-      <c r="F60" s="1"/>
-      <c r="G60" s="1"/>
+    <row r="60" spans="2:7" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B60" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="61" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B61" s="3"/>
@@ -1191,13 +1637,25 @@
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
     </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B62" s="3"/>
-      <c r="C62" s="1"/>
-      <c r="D62" s="1"/>
-      <c r="E62" s="1"/>
-      <c r="F62" s="1"/>
-      <c r="G62" s="1"/>
+    <row r="62" spans="2:7" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B62" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="63" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B63" s="3"/>
@@ -1207,13 +1665,25 @@
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
     </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B64" s="3"/>
-      <c r="C64" s="1"/>
-      <c r="D64" s="1"/>
-      <c r="E64" s="1"/>
-      <c r="F64" s="1"/>
-      <c r="G64" s="1"/>
+    <row r="64" spans="2:7" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B64" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B65" s="3"/>
@@ -1223,13 +1693,25 @@
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
     </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B66" s="3"/>
-      <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
-      <c r="E66" s="1"/>
-      <c r="F66" s="1"/>
-      <c r="G66" s="1"/>
+    <row r="66" spans="2:7" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B66" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="67" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B67" s="3"/>
@@ -1239,13 +1721,25 @@
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
     </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B68" s="3"/>
-      <c r="C68" s="1"/>
-      <c r="D68" s="1"/>
-      <c r="E68" s="1"/>
-      <c r="F68" s="1"/>
-      <c r="G68" s="1"/>
+    <row r="68" spans="2:7" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B68" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="69" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B69" s="3"/>
@@ -5279,6 +5773,94 @@
       <c r="F572" s="1"/>
       <c r="G572" s="1"/>
     </row>
+    <row r="573" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B573" s="3"/>
+      <c r="C573" s="1"/>
+      <c r="D573" s="1"/>
+      <c r="E573" s="1"/>
+      <c r="F573" s="1"/>
+      <c r="G573" s="1"/>
+    </row>
+    <row r="574" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B574" s="3"/>
+      <c r="C574" s="1"/>
+      <c r="D574" s="1"/>
+      <c r="E574" s="1"/>
+      <c r="F574" s="1"/>
+      <c r="G574" s="1"/>
+    </row>
+    <row r="575" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B575" s="3"/>
+      <c r="C575" s="1"/>
+      <c r="D575" s="1"/>
+      <c r="E575" s="1"/>
+      <c r="F575" s="1"/>
+      <c r="G575" s="1"/>
+    </row>
+    <row r="576" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B576" s="3"/>
+      <c r="C576" s="1"/>
+      <c r="D576" s="1"/>
+      <c r="E576" s="1"/>
+      <c r="F576" s="1"/>
+      <c r="G576" s="1"/>
+    </row>
+    <row r="577" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B577" s="3"/>
+      <c r="C577" s="1"/>
+      <c r="D577" s="1"/>
+      <c r="E577" s="1"/>
+      <c r="F577" s="1"/>
+      <c r="G577" s="1"/>
+    </row>
+    <row r="578" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B578" s="3"/>
+      <c r="C578" s="1"/>
+      <c r="D578" s="1"/>
+      <c r="E578" s="1"/>
+      <c r="F578" s="1"/>
+      <c r="G578" s="1"/>
+    </row>
+    <row r="579" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B579" s="3"/>
+      <c r="C579" s="1"/>
+      <c r="D579" s="1"/>
+      <c r="E579" s="1"/>
+      <c r="F579" s="1"/>
+      <c r="G579" s="1"/>
+    </row>
+    <row r="580" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B580" s="3"/>
+      <c r="C580" s="1"/>
+      <c r="D580" s="1"/>
+      <c r="E580" s="1"/>
+      <c r="F580" s="1"/>
+      <c r="G580" s="1"/>
+    </row>
+    <row r="581" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B581" s="3"/>
+      <c r="C581" s="1"/>
+      <c r="D581" s="1"/>
+      <c r="E581" s="1"/>
+      <c r="F581" s="1"/>
+      <c r="G581" s="1"/>
+    </row>
+    <row r="582" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B582" s="3"/>
+      <c r="C582" s="1"/>
+      <c r="D582" s="1"/>
+      <c r="E582" s="1"/>
+      <c r="F582" s="1"/>
+      <c r="G582" s="1"/>
+    </row>
+    <row r="583" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B583" s="3"/>
+      <c r="C583" s="1"/>
+      <c r="D583" s="1"/>
+      <c r="E583" s="1"/>
+      <c r="F583" s="1"/>
+      <c r="G583" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>

</xml_diff>